<commit_message>
it writes to excel all productList
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -372,7 +372,7 @@
     <t xml:space="preserve">Nº:01118601NN</t>
   </si>
   <si>
-    <t xml:space="preserve">Fecha:2020-03-21</t>
+    <t xml:space="preserve">Fecha:2020-03-19</t>
   </si>
   <si>
     <t xml:space="preserve">Naves</t>
@@ -424,6 +424,51 @@
   </si>
   <si>
     <t xml:space="preserve">HARINA DE CUARZO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DISOLVENTE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B a</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UNA MANO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C b</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <color rgb="FF0000"/>
+        <b/>
+        <sz val="12"/>
+      </rPr>
+      <t>GRISES</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="000000"/>
+        <b/>
+        <sz val="12"/>
+      </rPr>
+      <t xml:space="preserve"> 100% Sólidos (Primera y Segunda Mano)</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">SIN CARGO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D o</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E o</t>
   </si>
 </sst>
 </file>
@@ -780,6 +825,40 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+      <b/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFFFF"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFFFF"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FFFFFF"/>
+    </font>
   </fonts>
   <fills>
     <fill>
@@ -823,6 +902,27 @@
       </patternFill>
     </fill>
     <fill/>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF"/>
+      </patternFill>
+    </fill>
+    <fill/>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="0000FF"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders>
     <border>
@@ -1014,6 +1114,41 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1324,6 +1459,11 @@
     </xf>
     <xf numFmtId="0" fontId="46" fillId="7" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
     <xf numFmtId="0" fontId="47" fillId="8" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="48" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="49" fillId="10" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="50" fillId="11" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="12" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="52" fillId="13" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2563,7 +2703,9 @@
       </c>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="202"/>
+      <c r="B23" t="s" s="214">
+        <v>133</v>
+      </c>
       <c r="C23" s="202"/>
       <c r="D23" s="202"/>
       <c r="E23" s="209"/>
@@ -2572,16 +2714,26 @@
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="30"/>
-      <c r="C24" s="30"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="8"/>
+      <c r="B24" t="s" s="30">
+        <v>128</v>
+      </c>
+      <c r="C24" t="s" s="30">
+        <v>134</v>
+      </c>
+      <c r="D24" s="31">
+        <v>1</v>
+      </c>
+      <c r="E24" s="8">
+        <v>1</v>
+      </c>
       <c r="F24" s="8">
         <f t="shared" si="0"/>
       </c>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="30"/>
+      <c r="B25" t="s" s="215">
+        <v>135</v>
+      </c>
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
       <c r="E25" s="8"/>
@@ -2590,18 +2742,30 @@
       </c>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="202"/>
-      <c r="C26" s="202"/>
-      <c r="D26" s="202"/>
-      <c r="E26" s="209"/>
+      <c r="B26" t="s" s="202">
+        <v>128</v>
+      </c>
+      <c r="C26" t="s" s="202">
+        <v>136</v>
+      </c>
+      <c r="D26" s="202">
+        <v>2</v>
+      </c>
+      <c r="E26" s="209">
+        <v>1</v>
+      </c>
       <c r="F26" s="8">
         <f t="shared" si="0"/>
       </c>
       <c r="H26" s="198"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="30"/>
-      <c r="C27" s="210"/>
+      <c r="B27" t="s" s="216">
+        <v>130</v>
+      </c>
+      <c r="C27" t="s" s="210">
+        <v>137</v>
+      </c>
       <c r="D27" s="31"/>
       <c r="E27" s="8"/>
       <c r="F27" s="8">
@@ -2609,7 +2773,9 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="30"/>
+      <c r="B28" t="s" s="217">
+        <v>138</v>
+      </c>
       <c r="C28" s="30"/>
       <c r="D28" s="31"/>
       <c r="E28" s="8"/>
@@ -2618,16 +2784,26 @@
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="202"/>
-      <c r="C29" s="202"/>
-      <c r="D29" s="202"/>
-      <c r="E29" s="209"/>
+      <c r="B29" t="s" s="202">
+        <v>139</v>
+      </c>
+      <c r="C29" t="s" s="202">
+        <v>140</v>
+      </c>
+      <c r="D29" s="202">
+        <v>2</v>
+      </c>
+      <c r="E29" s="209">
+        <v>1</v>
+      </c>
       <c r="F29" s="8">
         <f t="shared" si="0"/>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="30"/>
+      <c r="B30" t="s" s="218">
+        <v>141</v>
+      </c>
       <c r="C30" s="30"/>
       <c r="D30" s="31"/>
       <c r="E30" s="8"/>
@@ -2636,10 +2812,18 @@
       </c>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="30"/>
-      <c r="C31" s="30"/>
-      <c r="D31" s="31"/>
-      <c r="E31" s="8"/>
+      <c r="B31" t="s" s="30">
+        <v>139</v>
+      </c>
+      <c r="C31" t="s" s="30">
+        <v>142</v>
+      </c>
+      <c r="D31" s="31">
+        <v>2</v>
+      </c>
+      <c r="E31" s="8">
+        <v>1</v>
+      </c>
       <c r="F31" s="8">
         <f t="shared" si="0"/>
       </c>
@@ -2707,7 +2891,7 @@
         <v>112</v>
       </c>
       <c r="D37" s="13">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E37" s="35">
         <v>0.33</v>

</xml_diff>

<commit_message>
file and folder opens when you create a new excel
</commit_message>
<xml_diff>
--- a/out.xlsx
+++ b/out.xlsx
@@ -369,10 +369,10 @@
     <t xml:space="preserve">Fecha: </t>
   </si>
   <si>
-    <t xml:space="preserve">Nº:01118601NN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fecha:2020-03-19</t>
+    <t xml:space="preserve">Nº:01118605RN</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fecha:2020-10-21</t>
   </si>
   <si>
     <t xml:space="preserve">Naves</t>
@@ -396,7 +396,7 @@
     <t xml:space="preserve">Spain</t>
   </si>
   <si>
-    <t xml:space="preserve">4567981</t>
+    <t xml:space="preserve">456798</t>
   </si>
   <si>
     <t xml:space="preserve">Mr. Demo</t>
@@ -414,7 +414,7 @@
     <t xml:space="preserve">a</t>
   </si>
   <si>
-    <t xml:space="preserve">YES maybe</t>
+    <t xml:space="preserve">A a</t>
   </si>
   <si>
     <t xml:space="preserve">Catalizador 5 a 1</t>
@@ -429,13 +429,13 @@
     <t xml:space="preserve">DISOLVENTE</t>
   </si>
   <si>
-    <t xml:space="preserve">B a</t>
-  </si>
-  <si>
     <t xml:space="preserve">UNA MANO</t>
   </si>
   <si>
-    <t xml:space="preserve">C b</t>
+    <t xml:space="preserve">c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C c</t>
   </si>
   <si>
     <r>
@@ -462,13 +462,10 @@
     <t xml:space="preserve">o</t>
   </si>
   <si>
-    <t xml:space="preserve">D o</t>
+    <t xml:space="preserve">O o</t>
   </si>
   <si>
     <t xml:space="preserve">3D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">E o</t>
   </si>
 </sst>
 </file>
@@ -846,6 +843,13 @@
       <family val="2"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="12"/>
       <name val="Calibri"/>
@@ -855,9 +859,10 @@
     <font>
       <b/>
       <sz val="12"/>
+      <color rgb="FFFFFF"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color rgb="FFFFFF"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills>
@@ -913,6 +918,9 @@
       </patternFill>
     </fill>
     <fill/>
+    <fill>
+      <patternFill patternType="none"/>
+    </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="0000FF"/>
@@ -1114,6 +1122,13 @@
       <bottom style="medium">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -1462,8 +1477,9 @@
     <xf numFmtId="0" fontId="48" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="49" fillId="10" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
     <xf numFmtId="0" fontId="50" fillId="11" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="51" fillId="12" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="51" fillId="12" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="52" fillId="13" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="53" fillId="14" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2665,10 +2681,10 @@
         <v>129</v>
       </c>
       <c r="D20" s="202">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="E20" s="209">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="F20" s="8">
         <f t="shared" ref="F20:F33" si="0">IF(D20&lt;&gt;"",D20*E20,"")</f>
@@ -2718,7 +2734,7 @@
         <v>128</v>
       </c>
       <c r="C24" t="s" s="30">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="D24" s="31">
         <v>1</v>
@@ -2732,7 +2748,7 @@
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" t="s" s="215">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C25" s="30"/>
       <c r="D25" s="31"/>
@@ -2743,16 +2759,16 @@
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" t="s" s="202">
-        <v>128</v>
+        <v>135</v>
       </c>
       <c r="C26" t="s" s="202">
         <v>136</v>
       </c>
       <c r="D26" s="202">
+        <v>3</v>
+      </c>
+      <c r="E26" s="209">
         <v>2</v>
-      </c>
-      <c r="E26" s="209">
-        <v>1</v>
       </c>
       <c r="F26" s="8">
         <f t="shared" si="0"/>
@@ -2773,36 +2789,38 @@
       </c>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" t="s" s="217">
-        <v>138</v>
-      </c>
-      <c r="C28" s="30"/>
-      <c r="D28" s="31"/>
-      <c r="E28" s="8"/>
+      <c r="B28" t="s" s="30">
+        <v>135</v>
+      </c>
+      <c r="C28" t="s" s="30">
+        <v>136</v>
+      </c>
+      <c r="D28" s="31">
+        <v>3</v>
+      </c>
+      <c r="E28" s="8">
+        <v>2</v>
+      </c>
       <c r="F28" s="8">
         <f t="shared" si="0"/>
       </c>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" t="s" s="202">
-        <v>139</v>
+      <c r="B29" t="s" s="217">
+        <v>130</v>
       </c>
       <c r="C29" t="s" s="202">
-        <v>140</v>
-      </c>
-      <c r="D29" s="202">
-        <v>2</v>
-      </c>
-      <c r="E29" s="209">
-        <v>1</v>
-      </c>
+        <v>137</v>
+      </c>
+      <c r="D29" s="202"/>
+      <c r="E29" s="209"/>
       <c r="F29" s="8">
         <f t="shared" si="0"/>
       </c>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" t="s" s="218">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="C30" s="30"/>
       <c r="D30" s="31"/>
@@ -2816,7 +2834,7 @@
         <v>139</v>
       </c>
       <c r="C31" t="s" s="30">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D31" s="31">
         <v>2</v>
@@ -2829,7 +2847,9 @@
       </c>
     </row>
     <row r="32" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="202"/>
+      <c r="B32" t="s" s="219">
+        <v>141</v>
+      </c>
       <c r="C32" s="202"/>
       <c r="D32" s="202"/>
       <c r="E32" s="209"/>
@@ -2838,10 +2858,18 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B33" s="30"/>
-      <c r="C33" s="210"/>
-      <c r="D33" s="31"/>
-      <c r="E33" s="8"/>
+      <c r="B33" t="s" s="30">
+        <v>139</v>
+      </c>
+      <c r="C33" t="s" s="210">
+        <v>140</v>
+      </c>
+      <c r="D33" s="31">
+        <v>2</v>
+      </c>
+      <c r="E33" s="8">
+        <v>1</v>
+      </c>
       <c r="F33" s="8">
         <f t="shared" si="0"/>
       </c>

</xml_diff>